<commit_message>
Mejora búsquedas en neteja y claus
</commit_message>
<xml_diff>
--- a/data/claus.xlsx
+++ b/data/claus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\_Flask_Python\gepV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCEED1B-8E86-4690-B24D-CABE2AAB903C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E55D28-150E-4258-B522-ED5AE9AA2220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33564" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{954C4DF0-A74D-403B-AE99-890BAE94F81F}"/>
+    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" xr2:uid="{954C4DF0-A74D-403B-AE99-890BAE94F81F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="213">
   <si>
     <t>Entrada + Campanar</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Dispensadors TORK</t>
   </si>
   <si>
-    <t>Entrada edifici. Vig. i Cap.</t>
-  </si>
-  <si>
     <t>GUARDIA MUNICIPAL</t>
   </si>
   <si>
@@ -149,27 +146,12 @@
     <t>Magatzem</t>
   </si>
   <si>
-    <t>Pack VIGILANS 01</t>
-  </si>
-  <si>
-    <t>Pack VIGILANS 02</t>
-  </si>
-  <si>
-    <t>Pack VIGILANS 03</t>
-  </si>
-  <si>
-    <t>Esq. Corredera urgencies</t>
-  </si>
-  <si>
     <t>CONSULTORI</t>
   </si>
   <si>
     <t>Acces posterior</t>
   </si>
   <si>
-    <t>Dreta corredera</t>
-  </si>
-  <si>
     <t>Quartet</t>
   </si>
   <si>
@@ -251,9 +233,6 @@
     <t>Persiana-Automatisme-Portes</t>
   </si>
   <si>
-    <t>P Vigilans i Cap</t>
-  </si>
-  <si>
     <t>P camp de futbol</t>
   </si>
   <si>
@@ -275,9 +254,6 @@
     <t>P Escola</t>
   </si>
   <si>
-    <t>P_Oficina del Parc</t>
-  </si>
-  <si>
     <t>ESCOLA BRESSOL</t>
   </si>
   <si>
@@ -293,12 +269,6 @@
     <t>Sala tècnica Poli</t>
   </si>
   <si>
-    <t>Vestuari 1</t>
-  </si>
-  <si>
-    <t>Vestuari 2</t>
-  </si>
-  <si>
     <t>Arbitre 1</t>
   </si>
   <si>
@@ -398,9 +368,6 @@
     <t>Originals la Llàntia</t>
   </si>
   <si>
-    <t>Porta terrasseta i Pack</t>
-  </si>
-  <si>
     <t>TERRASSETA BRIGADA</t>
   </si>
   <si>
@@ -446,9 +413,6 @@
     <t>WC</t>
   </si>
   <si>
-    <t>Portes riera Candau</t>
-  </si>
-  <si>
     <t>Porta Cementiri</t>
   </si>
   <si>
@@ -494,9 +458,6 @@
     <t>WC CANADA</t>
   </si>
   <si>
-    <t>Porta Pricipal</t>
-  </si>
-  <si>
     <t>DISCOTECA</t>
   </si>
   <si>
@@ -512,18 +473,12 @@
     <t>P La llàntia</t>
   </si>
   <si>
-    <t>P Diputació</t>
-  </si>
-  <si>
     <t>P Poliesportiu_Especial</t>
   </si>
   <si>
     <t>P Sala Expo</t>
   </si>
   <si>
-    <t>P Discoteca</t>
-  </si>
-  <si>
     <t>BiciTrail</t>
   </si>
   <si>
@@ -675,13 +630,58 @@
   </si>
   <si>
     <t>nom_espai</t>
+  </si>
+  <si>
+    <t>SERVEIS/CONSULTORI</t>
+  </si>
+  <si>
+    <t>P Serveis/Consultori</t>
+  </si>
+  <si>
+    <t>Porta drt. Consultori</t>
+  </si>
+  <si>
+    <t>Porta esq. Consultori</t>
+  </si>
+  <si>
+    <t>Entrada Consultori</t>
+  </si>
+  <si>
+    <t>CONSULTORI/SERVEIS</t>
+  </si>
+  <si>
+    <t>Automatisme</t>
+  </si>
+  <si>
+    <t>P Oficina del Park</t>
+  </si>
+  <si>
+    <t>P Consultori/Serveis</t>
+  </si>
+  <si>
+    <t>P Camp Futbool</t>
+  </si>
+  <si>
+    <t>Vestuari 1 dert</t>
+  </si>
+  <si>
+    <t>Vestuari 2 esq</t>
+  </si>
+  <si>
+    <t>Emergencia, principal, cuartet</t>
+  </si>
+  <si>
+    <t>Porta pricipal i pati gran</t>
+  </si>
+  <si>
+    <t>Contador llum 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,8 +712,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,6 +755,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -781,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -824,13 +843,32 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1167,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF8D717-D5CA-4BD4-8971-DA09B0A4DE2A}">
-  <dimension ref="A1:D199"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,16 +1220,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -1616,10 +1654,10 @@
     </row>
     <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>2</v>
@@ -1630,10 +1668,10 @@
     </row>
     <row r="33" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>2</v>
@@ -1644,10 +1682,10 @@
     </row>
     <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>2</v>
@@ -1657,53 +1695,53 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="8" t="s">
+      <c r="A35" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="14">
         <v>34</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D35" s="9">
-        <v>34</v>
-      </c>
     </row>
     <row r="36" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="6">
+      <c r="A36" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="14">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="9">
+      <c r="A37" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="26">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>2</v>
@@ -1714,10 +1752,10 @@
     </row>
     <row r="39" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>2</v>
@@ -1728,10 +1766,10 @@
     </row>
     <row r="40" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>2</v>
@@ -1742,10 +1780,10 @@
     </row>
     <row r="41" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>3</v>
+        <v>202</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>203</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>2</v>
@@ -1756,10 +1794,10 @@
     </row>
     <row r="42" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>2</v>
@@ -1770,10 +1808,10 @@
     </row>
     <row r="43" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>2</v>
@@ -1784,10 +1822,10 @@
     </row>
     <row r="44" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>2</v>
@@ -1798,10 +1836,10 @@
     </row>
     <row r="45" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>2</v>
@@ -1812,10 +1850,10 @@
     </row>
     <row r="46" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>2</v>
@@ -1826,10 +1864,10 @@
     </row>
     <row r="47" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>2</v>
@@ -1840,10 +1878,10 @@
     </row>
     <row r="48" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>2</v>
@@ -1854,10 +1892,10 @@
     </row>
     <row r="49" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>2</v>
@@ -1868,10 +1906,10 @@
     </row>
     <row r="50" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>2</v>
@@ -1882,10 +1920,10 @@
     </row>
     <row r="51" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>2</v>
@@ -1896,10 +1934,10 @@
     </row>
     <row r="52" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="C52" s="6" t="s">
         <v>2</v>
@@ -1910,10 +1948,10 @@
     </row>
     <row r="53" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>2</v>
@@ -1924,10 +1962,10 @@
     </row>
     <row r="54" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C54" s="6" t="s">
         <v>2</v>
@@ -1938,10 +1976,10 @@
     </row>
     <row r="55" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>2</v>
@@ -1952,10 +1990,10 @@
     </row>
     <row r="56" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>2</v>
@@ -1966,10 +2004,10 @@
     </row>
     <row r="57" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>2</v>
@@ -1980,10 +2018,10 @@
     </row>
     <row r="58" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>2</v>
@@ -1993,25 +2031,25 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D59" s="9">
+      <c r="A59" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="14">
         <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>2</v>
@@ -2022,10 +2060,10 @@
     </row>
     <row r="61" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>2</v>
@@ -2036,10 +2074,10 @@
     </row>
     <row r="62" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>2</v>
@@ -2050,1919 +2088,1947 @@
     </row>
     <row r="63" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>69</v>
+        <v>204</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="14">
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" s="6">
+    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="14">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D65" s="9">
+    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D66" s="14">
         <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66" s="6">
-        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D67" s="14">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D68" s="14">
-        <v>131</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B69" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D69" s="14">
-        <v>131</v>
+      <c r="A69" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="27">
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>72</v>
+        <v>205</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D70" s="14">
-        <v>133</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>75</v>
+        <v>205</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D71" s="14">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
-        <v>76</v>
+        <v>146</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D72" s="14">
-        <v>139</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>5</v>
+        <v>67</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D73" s="14">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>80</v>
+        <v>206</v>
+      </c>
+      <c r="B74" s="30" t="s">
+        <v>203</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="16">
-        <v>134</v>
+      <c r="D74" s="14">
+        <v>131</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D75" s="9">
-        <v>1</v>
+      <c r="A75" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="14">
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D76" s="6">
-        <v>2</v>
+      <c r="A76" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="16">
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D77" s="9">
-        <v>3</v>
+      <c r="A77" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="16">
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D78" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D79" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D80" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="11" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D81" s="9">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>88</v>
+        <v>208</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D82" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="11" t="s">
-        <v>89</v>
+        <v>209</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D83" s="9">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D84" s="6">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="11" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D85" s="9">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D86" s="6">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="11" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D87" s="9">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D88" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D91" s="9">
         <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D89" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D90" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="9">
-        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D92" s="6">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D93" s="9">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D94" s="6">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D95" s="9">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D96" s="6">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D97" s="9">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D98" s="6">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D99" s="9">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D100" s="6">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D101" s="9">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D102" s="6">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D103" s="9">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="10" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D104" s="6">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="11" t="s">
-        <v>112</v>
+      <c r="A105" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D105" s="9">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>113</v>
+      <c r="A106" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D106" s="6">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D107" s="9">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="10" t="s">
-        <v>115</v>
+      <c r="A108" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D108" s="6">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="7" t="s">
-        <v>117</v>
+      <c r="A109" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D109" s="9">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="10" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D110" s="6">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D111" s="9">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D112" s="14">
-        <v>38</v>
+      <c r="A112" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D112" s="6">
+        <v>35</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D113" s="9">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="10" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D114" s="6">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B115" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D115" s="9">
-        <v>41</v>
+      <c r="A115" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B115" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D115" s="14">
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D116" s="6">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D117" s="9">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D118" s="6">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>73</v>
+      <c r="A119" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D119" s="9">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="s">
-        <v>128</v>
+        <v>35</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D120" s="6">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>73</v>
+      <c r="A121" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D121" s="9">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D122" s="6">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>73</v>
+      <c r="A123" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D123" s="9">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D124" s="6">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>73</v>
+      <c r="A125" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D125" s="9">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="10" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D126" s="6">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D127" s="9">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="10" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D128" s="6">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D129" s="9">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="10" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D130" s="6">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D131" s="9">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="10" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D132" s="6">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D133" s="9">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="10" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D134" s="6">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D135" s="9">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="10" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D136" s="6">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D137" s="9">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="10" t="s">
-        <v>147</v>
+        <v>3</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D138" s="6">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D139" s="9">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="10" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D140" s="6">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D141" s="9">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="10" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D142" s="6">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D143" s="9">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="10" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D144" s="6">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
-        <v>156</v>
+        <v>211</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="C145" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D145" s="9">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="10" t="s">
-        <v>3</v>
+        <v>141</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D146" s="6">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
-        <v>3</v>
+        <v>142</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D147" s="9">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A148" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B148" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C148" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D148" s="14">
-        <v>104</v>
+      <c r="A148" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C148" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D148" s="6">
+        <v>71</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A149" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B149" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C149" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D149" s="14">
-        <v>106</v>
+      <c r="A149" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D149" s="9">
+        <v>72</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A150" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="B150" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C150" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D150" s="14">
-        <v>107</v>
+      <c r="A150" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D150" s="6">
+        <v>101</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="17" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D151" s="14">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="17" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D152" s="14">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="17" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D153" s="14">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="17" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D154" s="14">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A155" s="18" t="s">
-        <v>159</v>
-      </c>
-      <c r="B155" s="15" t="s">
-        <v>75</v>
+      <c r="A155" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B155" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D155" s="19">
-        <v>127</v>
+        <v>73</v>
+      </c>
+      <c r="D155" s="14">
+        <v>111</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="17" t="s">
-        <v>159</v>
+        <v>65</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D156" s="14">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="17" t="s">
-        <v>160</v>
+        <v>65</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D157" s="14">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A158" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="B158" s="13" t="s">
-        <v>106</v>
+      <c r="A158" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B158" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D158" s="14">
-        <v>133</v>
+        <v>73</v>
+      </c>
+      <c r="D158" s="19">
+        <v>127</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="17" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D159" s="14">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="17" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D160" s="14">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="17" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>153</v>
+        <v>96</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D161" s="14">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B162" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C162" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D162" s="14">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D163" s="14">
         <v>123</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A162" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C162" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D162" s="6">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A163" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B163" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C163" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D163" s="21" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row r="164" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A164" s="10" t="s">
-        <v>167</v>
+      <c r="A164" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C164" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D164" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C164" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D164" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C165" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D165" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C165" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D165" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A166" s="4" t="s">
-        <v>169</v>
+      <c r="A166" s="10" t="s">
+        <v>153</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C166" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D166" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C166" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D166" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="11" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C167" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D167" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C167" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D167" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C168" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D168" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C168" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D168" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="11" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C169" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D169" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C169" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D169" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C170" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D170" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C170" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D170" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A171" s="7" t="s">
-        <v>176</v>
+      <c r="A171" s="11" t="s">
+        <v>159</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C171" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D171" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C171" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D171" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="10" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="B172" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C172" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D172" s="22" t="s">
+      <c r="C172" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D172" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C173" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D173" s="21" t="s">
+      <c r="C173" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D173" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A174" s="4" t="s">
-        <v>179</v>
+      <c r="A174" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C174" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D174" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C174" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D174" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A175" s="7" t="s">
-        <v>180</v>
+      <c r="A175" s="11" t="s">
+        <v>164</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C175" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D175" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C175" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D175" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="10" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C176" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D176" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C176" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D176" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C177" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D177" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C177" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D177" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="10" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C178" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D178" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C178" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D178" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A179" s="11" t="s">
-        <v>185</v>
+      <c r="A179" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C179" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D179" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C179" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D179" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A180" s="10" t="s">
-        <v>186</v>
+      <c r="A180" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C180" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D180" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C180" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D180" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C181" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D181" s="21" t="s">
+      <c r="C181" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D181" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A182" s="4" t="s">
-        <v>188</v>
+      <c r="A182" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="B182" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C182" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D182" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D182" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A183" s="7" t="s">
-        <v>189</v>
+      <c r="A183" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C183" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D183" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C183" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D183" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="10" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B184" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C184" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D184" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D184" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="185" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="C185" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D185" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C185" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D185" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="10" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="B186" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C186" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D186" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C186" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D186" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A187" s="11" t="s">
-        <v>195</v>
+      <c r="A187" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C187" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D187" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C187" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D187" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B188" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C188" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D188" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D188" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A189" s="7" t="s">
-        <v>197</v>
+      <c r="A189" s="11" t="s">
+        <v>180</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C189" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D189" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C189" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D189" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="10" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C190" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D190" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C190" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D190" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C191" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D191" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C191" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D191" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A192" s="4" t="s">
-        <v>200</v>
+      <c r="A192" s="10" t="s">
+        <v>184</v>
       </c>
       <c r="B192" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C192" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D192" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D192" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="11" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C193" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D193" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C193" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D193" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A194" s="10" t="s">
-        <v>203</v>
+      <c r="A194" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="B194" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C194" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D194" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C194" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D194" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C195" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D195" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C195" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D195" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="10" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B196" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C196" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D196" s="22" t="s">
+      <c r="C196" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D196" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C197" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D197" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D197" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" s="10" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C198" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D198" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="C198" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D198" s="21" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C199" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="D199" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C199" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D199" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A200" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C200" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D200" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A201" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="D201" s="31" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>